<commit_message>
fix excel thành viên
</commit_message>
<xml_diff>
--- a/BiTech.Library/BiTech.Library/Tempaltes/MauSach.xlsx
+++ b/BiTech.Library/BiTech.Library/Tempaltes/MauSach.xlsx
@@ -612,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -994,6 +994,1014 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
+    <row r="19" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+    </row>
+    <row r="49" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+    </row>
+    <row r="51" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+    </row>
+    <row r="52" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+    </row>
+    <row r="53" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+    </row>
+    <row r="54" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+    </row>
+    <row r="55" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+    </row>
+    <row r="56" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+    </row>
+    <row r="57" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+    </row>
+    <row r="58" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+    </row>
+    <row r="59" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+    </row>
+    <row r="60" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+    </row>
+    <row r="61" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+    </row>
+    <row r="62" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+    </row>
+    <row r="63" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+    </row>
+    <row r="64" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+    </row>
+    <row r="65" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+    </row>
+    <row r="66" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+    </row>
+    <row r="67" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+    </row>
+    <row r="68" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+    </row>
+    <row r="69" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+    </row>
+    <row r="70" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+    </row>
+    <row r="71" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+    </row>
+    <row r="72" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+    </row>
+    <row r="73" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+    </row>
+    <row r="74" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>